<commit_message>
changing file structure of folder data
</commit_message>
<xml_diff>
--- a/fbref_league_ids.xlsx
+++ b/fbref_league_ids.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jan Jacobsen\DS_Tue_local\DS-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fb3b67440066c8ce/Jonah/Master/2_Semester/Data_Science_Project/DS-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ACE6E6-E90F-4F36-B9C8-7281ABDB6CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{A5ACE6E6-E90F-4F36-B9C8-7281ABDB6CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0445A824-8C46-4A37-B286-C38A38D0676B}"/>
   <bookViews>
-    <workbookView xWindow="3795" yWindow="3855" windowWidth="21600" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,14 +393,14 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +414,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>9</v>
       </c>
@@ -428,7 +428,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>12</v>
       </c>
@@ -442,7 +442,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>13</v>
       </c>
@@ -456,7 +456,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>20</v>
       </c>
@@ -470,7 +470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>11</v>
       </c>

</xml_diff>